<commit_message>
Added Time Slot Clash Handling
</commit_message>
<xml_diff>
--- a/code/courses_data/courses_2020_21.xlsx
+++ b/code/courses_data/courses_2020_21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HSS Course Allotment\HSS-Course-Allotment\code\courses_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20955CF4-5456-444D-A418-FCD16785F180}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4979B33D-51B8-4B4A-9EAD-E9B58CD331DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E897C076-3AD7-4959-BEFF-066CF231A49E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>Foundational Sanskrit</t>
   </si>
@@ -228,16 +228,58 @@
     <t>Course Code</t>
   </si>
   <si>
-    <t>Course Name</t>
-  </si>
-  <si>
-    <t>Course Cap</t>
-  </si>
-  <si>
     <t>HS 104</t>
   </si>
   <si>
     <t>HS 327</t>
+  </si>
+  <si>
+    <t>Course Title</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Time Slot Lecture</t>
+  </si>
+  <si>
+    <t>Time Slot Tutorial</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>K1</t>
   </si>
 </sst>
 </file>
@@ -298,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -321,6 +363,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36255BE9-FB71-406F-96D7-D5BA53CC48D8}">
   <dimension ref="A1:BY37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,21 +709,30 @@
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6">
         <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
@@ -709,6 +775,7 @@
       <c r="C3" s="6">
         <v>40</v>
       </c>
+      <c r="D3" s="11"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -750,6 +817,9 @@
       <c r="C4" s="6">
         <v>40</v>
       </c>
+      <c r="D4" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
@@ -791,6 +861,9 @@
       <c r="C5" s="6">
         <v>40</v>
       </c>
+      <c r="D5" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
@@ -832,6 +905,10 @@
       <c r="C6" s="6">
         <v>40</v>
       </c>
+      <c r="D6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="10"/>
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
@@ -873,6 +950,10 @@
       <c r="C7" s="6">
         <v>40</v>
       </c>
+      <c r="D7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
@@ -914,6 +995,10 @@
       <c r="C8" s="6">
         <v>40</v>
       </c>
+      <c r="D8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="10"/>
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
@@ -955,6 +1040,10 @@
       <c r="C9" s="6">
         <v>40</v>
       </c>
+      <c r="D9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
@@ -996,6 +1085,10 @@
       <c r="C10" s="6">
         <v>40</v>
       </c>
+      <c r="D10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="10"/>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
       <c r="AX10" s="1"/>
@@ -1037,6 +1130,10 @@
       <c r="C11" s="6">
         <v>40</v>
       </c>
+      <c r="D11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
       <c r="AX11" s="1"/>
@@ -1078,6 +1175,10 @@
       <c r="C12" s="6">
         <v>40</v>
       </c>
+      <c r="D12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
@@ -1119,6 +1220,8 @@
       <c r="C13" s="6">
         <v>40</v>
       </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
@@ -1160,6 +1263,8 @@
       <c r="C14" s="6">
         <v>40</v>
       </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
@@ -1201,6 +1306,10 @@
       <c r="C15" s="6">
         <v>40</v>
       </c>
+      <c r="D15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
@@ -1242,6 +1351,10 @@
       <c r="C16" s="6">
         <v>40</v>
       </c>
+      <c r="D16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="10"/>
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
@@ -1283,6 +1396,10 @@
       <c r="C17" s="6">
         <v>40</v>
       </c>
+      <c r="D17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="10"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
@@ -1324,6 +1441,10 @@
       <c r="C18" s="6">
         <v>40</v>
       </c>
+      <c r="D18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
       <c r="AX18" s="1"/>
@@ -1365,6 +1486,10 @@
       <c r="C19" s="6">
         <v>40</v>
       </c>
+      <c r="D19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="10"/>
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
@@ -1406,6 +1531,10 @@
       <c r="C20" s="6">
         <v>40</v>
       </c>
+      <c r="D20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="10"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
@@ -1447,6 +1576,10 @@
       <c r="C21" s="6">
         <v>40</v>
       </c>
+      <c r="D21" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
@@ -1488,6 +1621,10 @@
       <c r="C22" s="6">
         <v>40</v>
       </c>
+      <c r="D22" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="10"/>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
@@ -1529,6 +1666,10 @@
       <c r="C23" s="6">
         <v>40</v>
       </c>
+      <c r="D23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="10"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
@@ -1570,6 +1711,10 @@
       <c r="C24" s="6">
         <v>40</v>
       </c>
+      <c r="D24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
@@ -1611,6 +1756,10 @@
       <c r="C25" s="6">
         <v>30</v>
       </c>
+      <c r="D25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="10"/>
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
@@ -1652,6 +1801,12 @@
       <c r="C26" s="6">
         <v>40</v>
       </c>
+      <c r="D26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
@@ -1693,6 +1848,10 @@
       <c r="C27" s="6">
         <v>40</v>
       </c>
+      <c r="D27" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
       <c r="AX27" s="1"/>
@@ -1734,6 +1893,8 @@
       <c r="C28" s="6">
         <v>40</v>
       </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
@@ -1775,6 +1936,8 @@
       <c r="C29" s="6">
         <v>40</v>
       </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="10"/>
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
       <c r="AX29" s="1"/>
@@ -1816,6 +1979,8 @@
       <c r="C30" s="6">
         <v>40</v>
       </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
       <c r="AX30" s="1"/>
@@ -1849,7 +2014,7 @@
     </row>
     <row r="31" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
@@ -1857,6 +2022,7 @@
       <c r="C31" s="6">
         <v>40</v>
       </c>
+      <c r="E31" s="10"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
       <c r="AX31" s="1"/>
@@ -1898,6 +2064,8 @@
       <c r="C32" s="3">
         <v>40</v>
       </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
       <c r="AX32" s="1"/>
@@ -1939,6 +2107,8 @@
       <c r="C33" s="6">
         <v>40</v>
       </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
       <c r="AX33" s="1"/>

</xml_diff>